<commit_message>
Add missing value, when cell value isn't appended
</commit_message>
<xml_diff>
--- a/data/columns.xlsx
+++ b/data/columns.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hal/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hal/java/git/jtablesaw/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F14E2E9-95AE-1D40-BE5C-CF6BBC10D6EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D3387F-0F2B-9747-90F1-5C0707FDAC1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="11760" windowWidth="17340" windowHeight="9640" xr2:uid="{6AC5DA07-BDD9-6B41-BA60-19A5E2E869C2}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -97,7 +97,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +415,7 @@
   <dimension ref="B3:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:H5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixes #822 and #815 providing more extensive columntype options for readers (#909)
* Fix #822 and #815

* Apply PR requestes changes

* Changes asked in PR

* Rename variable for better code readibility
</commit_message>
<xml_diff>
--- a/data/columns.xlsx
+++ b/data/columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal\tablesaw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67C1435-E10A-4900-BD74-2BBB9C21111E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033ADCB3-C4A6-425D-8D28-097036C7D043}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58785" yWindow="1005" windowWidth="19140" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="3190" windowWidth="18280" windowHeight="8810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>stringcol</t>
   </si>
@@ -62,13 +62,17 @@
   <si>
     <t>Marit</t>
   </si>
+  <si>
+    <t>empty</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,12 +106,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,29 +329,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.4140625" customWidth="1"/>
+    <col min="1" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="7.75" customWidth="1"/>
     <col min="4" max="4" width="12.08203125" customWidth="1"/>
-    <col min="5" max="5" width="15.4140625" customWidth="1"/>
+    <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="9.25" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="10.4140625" customWidth="1"/>
-    <col min="10" max="26" width="8.58203125" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="10" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,8 +375,12 @@
       <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
@@ -399,7 +408,8 @@
         <v>135.34</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -427,19 +437,17 @@
         <v>137.35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Fix #751 and #882
Column type detection uses all column cells to determine the columnType instead of only the first one.
</commit_message>
<xml_diff>
--- a/data/columns.xlsx
+++ b/data/columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal\tablesaw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033ADCB3-C4A6-425D-8D28-097036C7D043}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCE3170-9023-49F1-9CA9-EDAF13E79FDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3190" windowWidth="18280" windowHeight="8810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59385" yWindow="1140" windowWidth="26145" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>stringcol</t>
   </si>
@@ -65,6 +65,21 @@
   <si>
     <t>empty</t>
   </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>mixed2</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>intcol2</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +87,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -329,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -348,9 +363,9 @@
     <col min="10" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +393,17 @@
       <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -404,11 +428,17 @@
         <v>43518.870937500003</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I5" si="0">C4+F4</f>
+        <f t="shared" ref="I4:I6" si="0">C4+F4</f>
         <v>135.34</v>
       </c>
+      <c r="K4" s="5">
+        <v>123</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -436,18 +466,57 @@
         <f t="shared" si="0"/>
         <v>137.35</v>
       </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>123</v>
+      </c>
+      <c r="M5">
+        <v>1234</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>125</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12345679</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12345678901</v>
+      </c>
+      <c r="F6" s="1">
+        <v>13.35</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>43913.913310185198</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>138.35</v>
+      </c>
+      <c r="M6">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1434,6 +1503,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix #751 and #882 (#931)
Column type detection uses all column cells to determine the columnType instead of only the first one.
</commit_message>
<xml_diff>
--- a/data/columns.xlsx
+++ b/data/columns.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\personal\tablesaw\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033ADCB3-C4A6-425D-8D28-097036C7D043}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCE3170-9023-49F1-9CA9-EDAF13E79FDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3190" windowWidth="18280" windowHeight="8810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="59385" yWindow="1140" windowWidth="26145" windowHeight="12150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>stringcol</t>
   </si>
@@ -65,6 +65,21 @@
   <si>
     <t>empty</t>
   </si>
+  <si>
+    <t>mixed</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>mixed2</t>
+  </si>
+  <si>
+    <t>Quentin</t>
+  </si>
+  <si>
+    <t>intcol2</t>
+  </si>
 </sst>
 </file>
 
@@ -72,7 +87,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;$&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -329,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -348,9 +363,9 @@
     <col min="10" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -378,8 +393,17 @@
       <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="K3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -404,11 +428,17 @@
         <v>43518.870937500003</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" ref="I4:I5" si="0">C4+F4</f>
+        <f t="shared" ref="I4:I6" si="0">C4+F4</f>
         <v>135.34</v>
       </c>
+      <c r="K4" s="5">
+        <v>123</v>
+      </c>
+      <c r="L4" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -436,18 +466,57 @@
         <f t="shared" si="0"/>
         <v>137.35</v>
       </c>
+      <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>123</v>
+      </c>
+      <c r="M5">
+        <v>1234</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:13" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>125</v>
+      </c>
+      <c r="D6" s="1">
+        <v>12345679</v>
+      </c>
+      <c r="E6" s="1">
+        <v>12345678901</v>
+      </c>
+      <c r="F6" s="1">
+        <v>13.35</v>
+      </c>
+      <c r="G6" s="2" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>43913.913310185198</v>
+      </c>
+      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>138.35</v>
+      </c>
+      <c r="M6">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1434,6 +1503,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>